<commit_message>
Slut-statusrapport. Mangler opdateret WBS
</commit_message>
<xml_diff>
--- a/reports/r8/opfolgning.xlsx
+++ b/reports/r8/opfolgning.xlsx
@@ -4,25 +4,26 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="9270" windowHeight="4665" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="9270" windowHeight="4665" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Opfølgning" sheetId="1" r:id="rId1"/>
     <sheet name="Tidsregnskab" sheetId="2" r:id="rId2"/>
     <sheet name="kvalitet" sheetId="6" r:id="rId3"/>
     <sheet name="Ressourcer" sheetId="3" r:id="rId4"/>
-    <sheet name="status 13-6" sheetId="9" r:id="rId5"/>
-    <sheet name="status 05-6" sheetId="8" r:id="rId6"/>
-    <sheet name="status 30-5" sheetId="7" r:id="rId7"/>
-    <sheet name="status 30-3" sheetId="5" r:id="rId8"/>
-    <sheet name="status" sheetId="4" r:id="rId9"/>
+    <sheet name="status 15-6" sheetId="10" r:id="rId5"/>
+    <sheet name="status 13-6" sheetId="9" r:id="rId6"/>
+    <sheet name="status 05-6" sheetId="8" r:id="rId7"/>
+    <sheet name="status 30-5" sheetId="7" r:id="rId8"/>
+    <sheet name="status 30-3" sheetId="5" r:id="rId9"/>
+    <sheet name="status" sheetId="4" r:id="rId10"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="105">
   <si>
     <t>Forbrugt kal. til dato</t>
   </si>
@@ -328,6 +329,15 @@
   </si>
   <si>
     <t>Status 4</t>
+  </si>
+  <si>
+    <t>CDIO-konference</t>
+  </si>
+  <si>
+    <t>Eksamen</t>
+  </si>
+  <si>
+    <t>Konkurrence (se oven)</t>
   </si>
 </sst>
 </file>
@@ -838,15 +848,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.140625" customWidth="1"/>
     <col min="2" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="14" width="9.7109375" customWidth="1"/>
+    <col min="10" max="12" width="9.7109375" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" customWidth="1"/>
     <col min="15" max="15" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1044,35 +1056,35 @@
         <v>60</v>
       </c>
       <c r="H6" s="18">
-        <f t="shared" ref="H6:O6" si="0">$O1-H1</f>
+        <f>$O1-H1</f>
         <v>36</v>
       </c>
       <c r="I6" s="18">
-        <f t="shared" si="0"/>
+        <f>$O1-I1</f>
         <v>25</v>
       </c>
       <c r="J6" s="11">
-        <f t="shared" si="0"/>
+        <f>$O1-J1</f>
         <v>18</v>
       </c>
       <c r="K6" s="11">
-        <f t="shared" si="0"/>
+        <f>$O1-K1</f>
         <v>10</v>
       </c>
       <c r="L6" s="11">
-        <f t="shared" si="0"/>
+        <f>$O1-L1</f>
         <v>9</v>
       </c>
       <c r="M6" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="M6" si="0">$O1-M1</f>
         <v>7</v>
       </c>
       <c r="N6" s="20">
-        <f t="shared" si="0"/>
+        <f>$O1-N1</f>
         <v>4</v>
       </c>
       <c r="O6" s="18">
-        <f t="shared" si="0"/>
+        <f>$O1-O1</f>
         <v>0</v>
       </c>
     </row>
@@ -1251,10 +1263,16 @@
         <f>'status 13-6'!$A$1*100</f>
         <v>74.993055555555571</v>
       </c>
-      <c r="L11" s="11"/>
+      <c r="L11" s="11">
+        <v>77</v>
+      </c>
       <c r="M11" s="11"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="18"/>
+      <c r="N11" s="20">
+        <v>87</v>
+      </c>
+      <c r="O11" s="18">
+        <v>95</v>
+      </c>
     </row>
     <row r="12" spans="1:15">
       <c r="B12" s="17"/>
@@ -1357,12 +1375,18 @@
       </c>
       <c r="K14" s="34">
         <f>kvalitet!$E$2*100</f>
-        <v>66.875</v>
-      </c>
-      <c r="L14" s="11"/>
+        <v>93.958333333333343</v>
+      </c>
+      <c r="L14" s="11">
+        <v>69</v>
+      </c>
       <c r="M14" s="11"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="18"/>
+      <c r="N14" s="20">
+        <v>90</v>
+      </c>
+      <c r="O14" s="18">
+        <v>94</v>
+      </c>
     </row>
     <row r="15" spans="1:15">
       <c r="B15" s="17"/>
@@ -1482,10 +1506,18 @@
         <f>$B$17*(100-K11)/100</f>
         <v>191.30312499999988</v>
       </c>
-      <c r="L17" s="11"/>
+      <c r="L17" s="11">
+        <f>$B$17*(100-L11)/100</f>
+        <v>175.95</v>
+      </c>
       <c r="M17" s="11"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="18"/>
+      <c r="N17" s="11">
+        <f>$B$17*(100-N11)/100</f>
+        <v>99.45</v>
+      </c>
+      <c r="O17" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="1" t="s">
@@ -1521,10 +1553,16 @@
       <c r="K18" s="11">
         <v>613</v>
       </c>
-      <c r="L18" s="11"/>
+      <c r="L18" s="11">
+        <v>686</v>
+      </c>
       <c r="M18" s="11"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="18"/>
+      <c r="N18" s="20">
+        <v>885</v>
+      </c>
+      <c r="O18" s="18">
+        <v>974</v>
+      </c>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" t="s">
@@ -1565,12 +1603,351 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="30">
+        <f>B2*D2+B26*D26</f>
+        <v>0.5573611111111112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" s="30">
+        <f>C3*E3+C16*E16+C22*E22</f>
+        <v>0.91472222222222244</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" s="30"/>
+      <c r="C3" s="31">
+        <f>D4*F4+D6*F6+D9*F9+D13*F13</f>
+        <v>0.91250000000000009</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="D4" s="31">
+        <f>E5*G5</f>
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="E5" s="31">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="D6" s="31">
+        <f>E7*G7+E8*G8</f>
+        <v>0.85000000000000009</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="E7" s="31">
+        <v>0.9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="E8" s="31">
+        <v>0.8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="D9" s="31">
+        <f>E10*G10+E11*G11+E12*G12</f>
+        <v>0.85</v>
+      </c>
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="E10" s="31">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="E11" s="31">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="E12" s="31">
+        <v>0.7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="D13" s="31">
+        <f>E14*G14+E15*G15</f>
+        <v>0.95</v>
+      </c>
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="E14" s="31">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="E15" s="31">
+        <v>0.9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="C16" s="31">
+        <f>D17*F17+D18*F18+D21*F21</f>
+        <v>0.96500000000000008</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="D17" s="31">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="31">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="D18" s="31">
+        <f>E19*G19+E20*G20</f>
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="31">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="E19" s="31">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="E20" s="31">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="D21" s="31">
+        <v>0.7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="31">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="C22">
+        <f>D23*F23+D24*F24+D25*F25</f>
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="D23" s="31">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="D24" s="31">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="D25" s="31">
+        <v>0.6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="31">
+        <f>C27*E27</f>
+        <v>0.2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="C27" s="31">
+        <f>D28*F28</f>
+        <v>0.2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="D28" s="31">
+        <v>0.2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="31">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1584,7 +1961,7 @@
     <col min="8" max="8" width="3" style="27" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="3" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -2278,6 +2655,91 @@
       </c>
       <c r="K32">
         <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="29">
+        <v>40714</v>
+      </c>
+      <c r="L33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="29">
+        <v>40715</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="L34" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="29">
+        <v>40716</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="G35">
+        <v>4</v>
+      </c>
+      <c r="I35">
+        <v>4</v>
+      </c>
+      <c r="K35">
+        <v>4</v>
+      </c>
+      <c r="L35" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="29">
+        <v>40717</v>
+      </c>
+      <c r="C36">
+        <v>8</v>
+      </c>
+      <c r="E36">
+        <v>8</v>
+      </c>
+      <c r="G36">
+        <v>7</v>
+      </c>
+      <c r="I36">
+        <v>8</v>
+      </c>
+      <c r="K36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="29">
+        <v>40718</v>
+      </c>
+      <c r="C37">
+        <v>5</v>
+      </c>
+      <c r="E37">
+        <v>5</v>
+      </c>
+      <c r="G37">
+        <v>5</v>
+      </c>
+      <c r="I37">
+        <v>5</v>
+      </c>
+      <c r="K37">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2298,8 +2760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2324,11 +2786,11 @@
       </c>
       <c r="D2" s="31">
         <f>D4*$C$4+D9*$C$9</f>
-        <v>0.6635416666666667</v>
+        <v>1</v>
       </c>
       <c r="E2" s="31">
         <f>E4*$C$4+E9*$C$9</f>
-        <v>0.66874999999999996</v>
+        <v>0.93958333333333344</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2372,11 +2834,11 @@
       </c>
       <c r="D9" s="31">
         <f>D10*$C$10+D28*$C$28</f>
-        <v>0.55138888888888893</v>
+        <v>1</v>
       </c>
       <c r="E9" s="31">
         <f>E10*$C$10+E28*$C$28</f>
-        <v>0.55833333333333335</v>
+        <v>0.91944444444444451</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2388,11 +2850,11 @@
       </c>
       <c r="D10" s="31">
         <f>D11*$C$11+D15*$C$15+D23*$C$23</f>
-        <v>0.60277777777777775</v>
+        <v>1</v>
       </c>
       <c r="E10" s="31">
         <f>E11*$C$11+E15*$C$15+E23*$C$23</f>
-        <v>0.66666666666666663</v>
+        <v>0.93888888888888888</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2405,11 +2867,11 @@
       </c>
       <c r="D11" s="31">
         <f>AVERAGE(D12:D13)</f>
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E11" s="31">
         <f>AVERAGE(E12:E13)</f>
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2417,10 +2879,10 @@
         <v>75</v>
       </c>
       <c r="D12" s="31">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E12" s="31">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2428,10 +2890,10 @@
         <v>96</v>
       </c>
       <c r="D13" s="31">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E13" s="31">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2444,11 +2906,11 @@
       </c>
       <c r="D15" s="31">
         <f>AVERAGE(D16:D21)</f>
-        <v>0.70833333333333337</v>
+        <v>1</v>
       </c>
       <c r="E15" s="31">
         <f>AVERAGE(E16:E21)</f>
-        <v>0.75</v>
+        <v>0.98333333333333339</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -2456,10 +2918,10 @@
         <v>79</v>
       </c>
       <c r="D16" s="31">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E16" s="31">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2467,10 +2929,10 @@
         <v>76</v>
       </c>
       <c r="D17" s="31">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E17" s="31">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2478,10 +2940,10 @@
         <v>77</v>
       </c>
       <c r="D18" s="31">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E18" s="31">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2489,10 +2951,10 @@
         <v>78</v>
       </c>
       <c r="D19" s="31">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E19" s="31">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -2500,10 +2962,10 @@
         <v>94</v>
       </c>
       <c r="D20" s="31">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E20" s="31">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -2511,10 +2973,10 @@
         <v>95</v>
       </c>
       <c r="D21" s="31">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E21" s="31">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2527,11 +2989,11 @@
       </c>
       <c r="D23" s="31">
         <f>AVERAGE(D24:D26)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E23" s="31">
         <f>AVERAGE(E24:E26)</f>
-        <v>0.75</v>
+        <v>0.93333333333333324</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2539,10 +3001,10 @@
         <v>80</v>
       </c>
       <c r="D24" s="31">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E24" s="31">
-        <v>0.75</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2550,10 +3012,10 @@
         <v>81</v>
       </c>
       <c r="D25" s="31">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E25" s="31">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2561,10 +3023,10 @@
         <v>82</v>
       </c>
       <c r="D26" s="31">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E26" s="31">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -2576,11 +3038,11 @@
       </c>
       <c r="D28" s="31">
         <f>AVERAGE(D29:D30)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E28" s="31">
         <f>AVERAGE(E29:E30)</f>
-        <v>0.45</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -2588,10 +3050,10 @@
         <v>84</v>
       </c>
       <c r="D29" s="31">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E29" s="31">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -2599,10 +3061,10 @@
         <v>83</v>
       </c>
       <c r="D30" s="31">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E30" s="31">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
@@ -2839,7 +3301,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2853,7 +3315,7 @@
         <v>71</v>
       </c>
       <c r="G1" s="29">
-        <v>40699</v>
+        <v>40709</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -3177,6 +3639,348 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="30">
+        <f>B2*D2+B26*D26</f>
+        <v>0.74993055555555566</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="29">
+        <v>40707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" s="30">
+        <f>C3*E3+C16*E16+C22*E22</f>
+        <v>0.94986111111111127</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" s="30"/>
+      <c r="C3" s="31">
+        <f>D4*F4+D6*F6+D9*F9+D13*F13</f>
+        <v>0.95625000000000004</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="D4" s="31">
+        <f>E5*G5</f>
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="E5" s="31">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="D6" s="31">
+        <f>E7*G7+E8*G8</f>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="E7" s="31">
+        <v>0.95</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="E8" s="31">
+        <v>0.9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="D9" s="31">
+        <f>E10*G10+E11*G11+E12*G12</f>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="E10" s="31">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="E11" s="31">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="E12" s="31">
+        <v>0.85</v>
+      </c>
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="D13" s="31">
+        <f>E14*G14+E15*G15</f>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="E14" s="31">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="E15" s="31">
+        <v>0.95</v>
+      </c>
+      <c r="F15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="C16" s="31">
+        <f>D17*F17+D18*F18+D21*F21</f>
+        <v>0.96000000000000019</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="D17" s="31">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="31">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="D18" s="31">
+        <f>E19*G19+E20*G20</f>
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="31">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="E19" s="31">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="E20" s="31">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="D21" s="31">
+        <v>0.9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="31">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="C22">
+        <f>D23*F23+D24*F24+D25*F25</f>
+        <v>0.93333333333333346</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="D23" s="31">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="D24" s="31">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="D25" s="31">
+        <v>0.8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="31">
+        <f>C27*E27</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="C27" s="31">
+        <f>D28*F28</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D27" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="D28" s="31">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E28" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="31">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -3518,7 +4322,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -3857,7 +4661,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -4195,343 +4999,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="30">
-        <f>B2*D2+B26*D26</f>
-        <v>0.5573611111111112</v>
-      </c>
-      <c r="B1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="B2" s="30">
-        <f>C3*E3+C16*E16+C22*E22</f>
-        <v>0.91472222222222244</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="31">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="B3" s="30"/>
-      <c r="C3" s="31">
-        <f>D4*F4+D6*F6+D9*F9+D13*F13</f>
-        <v>0.91250000000000009</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3">
-        <f>(100/3)%</f>
-        <v>0.33333333333333337</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="D4" s="31">
-        <f>E5*G5</f>
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="31">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="E5" s="31">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="D6" s="31">
-        <f>E7*G7+E8*G8</f>
-        <v>0.85000000000000009</v>
-      </c>
-      <c r="E6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="31">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="E7" s="31">
-        <v>0.9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="31">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="E8" s="31">
-        <v>0.8</v>
-      </c>
-      <c r="F8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="31">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="D9" s="31">
-        <f>E10*G10+E11*G11+E12*G12</f>
-        <v>0.85</v>
-      </c>
-      <c r="E9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="31">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="E10" s="31">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="31">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="E11" s="31">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="31">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="E12" s="31">
-        <v>0.7</v>
-      </c>
-      <c r="F12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="31">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="D13" s="31">
-        <f>E14*G14+E15*G15</f>
-        <v>0.95</v>
-      </c>
-      <c r="E13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="31">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="E14" s="31">
-        <v>1</v>
-      </c>
-      <c r="F14" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="31">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="E15" s="31">
-        <v>0.9</v>
-      </c>
-      <c r="F15" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="31">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="C16" s="31">
-        <f>D17*F17+D18*F18+D21*F21</f>
-        <v>0.96500000000000008</v>
-      </c>
-      <c r="D16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16">
-        <f>(100/3)%</f>
-        <v>0.33333333333333337</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="D17" s="31">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="31">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="D18" s="31">
-        <f>E19*G19+E20*G20</f>
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="31">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="E19" s="31">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" s="31">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="E20" s="31">
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" s="31">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="D21" s="31">
-        <v>0.7</v>
-      </c>
-      <c r="E21" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="31">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="C22">
-        <f>D23*F23+D24*F24+D25*F25</f>
-        <v>0.8666666666666667</v>
-      </c>
-      <c r="D22" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22">
-        <f>(100/3)%</f>
-        <v>0.33333333333333337</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="D23" s="31">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>66</v>
-      </c>
-      <c r="F23">
-        <f>(100/3)%</f>
-        <v>0.33333333333333337</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="D24" s="31">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24">
-        <f>(100/3)%</f>
-        <v>0.33333333333333337</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7">
-      <c r="D25" s="31">
-        <v>0.6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>58</v>
-      </c>
-      <c r="F25">
-        <f>(100/3)%</f>
-        <v>0.33333333333333337</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7">
-      <c r="B26" s="31">
-        <f>C27*E27</f>
-        <v>0.2</v>
-      </c>
-      <c r="C26" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="31">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7">
-      <c r="C27" s="31">
-        <f>D28*F28</f>
-        <v>0.2</v>
-      </c>
-      <c r="D27" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7">
-      <c r="D28" s="31">
-        <v>0.2</v>
-      </c>
-      <c r="E28" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" s="31">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>